<commit_message>
update : sửa file excel của danh sách nhân viên
sửa file excel của danh sách nhân viên cho bố cục rõ ràng
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/Brief/Danh-sách-nhân-viên.xlsx
+++ b/QUANGHANH2/excel/TCLD/Brief/Danh-sách-nhân-viên.xlsx
@@ -19,33 +19,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+  <si>
+    <t>STT</t>
+  </si>
   <si>
     <t>Mã Nhân viên</t>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t xml:space="preserve">Họ và tên </t>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Giới tính</t>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Ngày sinh</t>
-    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Số CMND</t>
   </si>
   <si>
     <t xml:space="preserve">Số sổ BHXH </t>
   </si>
   <si>
+    <t>Quá trình công việc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ngày đi làm </t>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Số năm đi làm</t>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Trình độ</t>
@@ -55,58 +58,6 @@
   </si>
   <si>
     <t>Quê quán</t>
-  </si>
-  <si>
-    <t>Số CMND</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Quá trình công việc</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Đơn vị</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Công việc</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Bậc</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Mức lương</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Thang lương</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Bậc</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Công việc hiện tại</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Đơn vị</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Công việc</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Mức lương</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>STT</t>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <r>
@@ -125,19 +76,37 @@
     </r>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>Công việc hiện tại</t>
+  </si>
+  <si>
+    <t>Đơn vị</t>
+  </si>
+  <si>
+    <t>Công việc</t>
+  </si>
+  <si>
+    <t>Mức lương</t>
+  </si>
+  <si>
+    <t>Thang lương</t>
+  </si>
+  <si>
+    <t>Bậc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -153,21 +122,6 @@
       <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="MS PMincho"/>
-      <family val="1"/>
-      <charset val="128"/>
     </font>
     <font>
       <b/>
@@ -187,6 +141,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="MS PMincho"/>
+      <family val="1"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -268,41 +230,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -582,158 +544,159 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="72.88671875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19" style="3" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="25.44140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="78.44140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="20.21875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" style="3" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.796875" style="1"/>
+    <col min="20" max="20" width="13.77734375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.77734375" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="3" customFormat="1">
-      <c r="A1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="U1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>9</v>
+      <c r="V1" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="10" customFormat="1" ht="17.399999999999999">
-      <c r="A2" s="11"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
+    <row r="2" spans="1:22" s="4" customFormat="1" ht="19.8">
+      <c r="A2" s="9"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="P3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -742,16 +705,16 @@
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="B1:B3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="H1:Q1"/>
     <mergeCell ref="G1:G3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TCLD - [fix] EmployeeController export excel
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/Brief/Danh-sách-nhân-viên.xlsx
+++ b/QUANGHANH2/excel/TCLD/Brief/Danh-sách-nhân-viên.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -241,6 +241,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -250,16 +259,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -542,126 +542,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="153.109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="19" style="3" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="25.44140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="78.44140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="31.77734375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="32.21875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="19.88671875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.5546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="45.77734375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="94.77734375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="8.77734375" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="45.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="153.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="78.42578125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="31.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="32.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="45.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="94.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="3" customFormat="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:19" s="3" customFormat="1">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="P1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="Q1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="R1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="S1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="4" customFormat="1" ht="19.8">
-      <c r="A2" s="6"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9" t="s">
+    <row r="2" spans="1:19" s="4" customFormat="1" ht="19.5">
+      <c r="A2" s="9"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
     </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="7"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
+    <row r="3" spans="1:19">
+      <c r="A3" s="10"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
@@ -669,52 +660,43 @@
         <v>16</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="9"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="H1:Q1"/>
-    <mergeCell ref="G1:G3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="B1:B3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="G1:G3"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>